<commit_message>
Enhance e_cef_extratos function by introducing a new variable for PJ and Repasse categorization; update document references for improved data processing. Modify e_cef_ecns function to identify the most recent ECN file for better data extraction.
</commit_message>
<xml_diff>
--- a/dados/2419 Estação jan-mar.xlsx
+++ b/dados/2419 Estação jan-mar.xlsx
@@ -31155,8 +31155,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006C56FB2846673243A9735D5EC6051572" ma:contentTypeVersion="11" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="941ba21155b641a9d77936be19967558">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5a5f483f-f768-438e-b4ef-63f46a7558dd" xmlns:ns3="dd8c73df-45bd-468c-aae5-f3faedcbd5e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="469d177505629adaca6589b93d36bf5c" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006C56FB2846673243A9735D5EC6051572" ma:contentTypeVersion="11" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="36569ac63cfce8ff0f8884bc80e67f1c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5a5f483f-f768-438e-b4ef-63f46a7558dd" xmlns:ns3="dd8c73df-45bd-468c-aae5-f3faedcbd5e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2040da04b75a9ea4fe796fa8180f8ca6" ns2:_="" ns3:_="">
     <xsd:import namespace="5a5f483f-f768-438e-b4ef-63f46a7558dd"/>
     <xsd:import namespace="dd8c73df-45bd-468c-aae5-f3faedcbd5e2"/>
     <xsd:element name="properties">
@@ -31369,22 +31369,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70D88B59-3506-486D-AA57-971AB028899C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5a5f483f-f768-438e-b4ef-63f46a7558dd"/>
-    <ds:schemaRef ds:uri="dd8c73df-45bd-468c-aae5-f3faedcbd5e2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7459D5F1-F939-4A08-8E26-C823ABFB4D8B}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>